<commit_message>
Fix excel orderforms (#4177)
Closes #4143
Fix excel order fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.33.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.33.balsamic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isakohlsson/dev/cg/tests/fixtures/orderforms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsdiazboada/Documents/Clinical_Genomics/repos/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DA0162F-BF7E-D645-B220-A87160CE58D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9997AFDC-8780-7F46-9F69-0323F61D69C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-13500" windowWidth="25560" windowHeight="28320" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="851">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -5923,8 +5923,8 @@
   </sheetPr>
   <dimension ref="A1:AMO395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AF16" sqref="AF16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -13625,7 +13625,7 @@
         <v>724</v>
       </c>
       <c r="F15" s="67" t="s">
-        <v>78</v>
+        <v>606</v>
       </c>
       <c r="G15" s="68" t="s">
         <v>68</v>
@@ -13659,7 +13659,9 @@
         <v>75</v>
       </c>
       <c r="R15" s="74"/>
-      <c r="S15" s="73"/>
+      <c r="S15" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U15" s="88"/>
       <c r="V15" s="102"/>
       <c r="W15" s="65"/>
@@ -15745,7 +15747,7 @@
         <v>730</v>
       </c>
       <c r="F17" s="67" t="s">
-        <v>89</v>
+        <v>606</v>
       </c>
       <c r="G17" s="68" t="s">
         <v>79</v>
@@ -15775,7 +15777,9 @@
       <c r="P17" s="70"/>
       <c r="Q17" s="85"/>
       <c r="R17" s="74"/>
-      <c r="S17" s="73"/>
+      <c r="S17" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U17" s="88"/>
       <c r="V17" s="102"/>
       <c r="W17" s="141"/>
@@ -16802,7 +16806,7 @@
         <v>733</v>
       </c>
       <c r="F18" s="67" t="s">
-        <v>89</v>
+        <v>606</v>
       </c>
       <c r="G18" s="68" t="s">
         <v>79</v>
@@ -16832,7 +16836,9 @@
       <c r="P18" s="70"/>
       <c r="Q18" s="85"/>
       <c r="R18" s="74"/>
-      <c r="S18" s="73"/>
+      <c r="S18" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U18" s="88"/>
       <c r="V18" s="102"/>
       <c r="W18" s="141"/>
@@ -17859,7 +17865,7 @@
         <v>736</v>
       </c>
       <c r="F19" s="67" t="s">
-        <v>453</v>
+        <v>607</v>
       </c>
       <c r="G19" s="68" t="s">
         <v>79</v>
@@ -17889,7 +17895,9 @@
       <c r="P19" s="70"/>
       <c r="Q19" s="85"/>
       <c r="R19" s="74"/>
-      <c r="S19" s="73"/>
+      <c r="S19" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U19" s="88"/>
       <c r="V19" s="102"/>
       <c r="W19" s="141"/>
@@ -18916,7 +18924,7 @@
         <v>739</v>
       </c>
       <c r="F20" s="67" t="s">
-        <v>470</v>
+        <v>607</v>
       </c>
       <c r="G20" s="68" t="s">
         <v>79</v>
@@ -18946,7 +18954,9 @@
       <c r="P20" s="70"/>
       <c r="Q20" s="85"/>
       <c r="R20" s="74"/>
-      <c r="S20" s="73"/>
+      <c r="S20" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U20" s="88"/>
       <c r="V20" s="102"/>
       <c r="W20" s="141"/>
@@ -19973,7 +19983,7 @@
         <v>742</v>
       </c>
       <c r="F21" s="67" t="s">
-        <v>470</v>
+        <v>607</v>
       </c>
       <c r="G21" s="68" t="s">
         <v>79</v>
@@ -20003,7 +20013,9 @@
       <c r="P21" s="70"/>
       <c r="Q21" s="85"/>
       <c r="R21" s="74"/>
-      <c r="S21" s="73"/>
+      <c r="S21" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U21" s="88"/>
       <c r="V21" s="102"/>
       <c r="W21" s="141"/>
@@ -21030,7 +21042,7 @@
         <v>745</v>
       </c>
       <c r="F22" s="67" t="s">
-        <v>454</v>
+        <v>608</v>
       </c>
       <c r="G22" s="68" t="s">
         <v>79</v>
@@ -21060,7 +21072,9 @@
       <c r="P22" s="70"/>
       <c r="Q22" s="85"/>
       <c r="R22" s="74"/>
-      <c r="S22" s="73"/>
+      <c r="S22" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U22" s="88"/>
       <c r="V22" s="102"/>
       <c r="W22" s="141"/>
@@ -22087,7 +22101,7 @@
         <v>748</v>
       </c>
       <c r="F23" s="67" t="s">
-        <v>455</v>
+        <v>607</v>
       </c>
       <c r="G23" s="68" t="s">
         <v>79</v>
@@ -22117,7 +22131,9 @@
       <c r="P23" s="70"/>
       <c r="Q23" s="85"/>
       <c r="R23" s="74"/>
-      <c r="S23" s="73"/>
+      <c r="S23" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U23" s="88"/>
       <c r="V23" s="102"/>
       <c r="W23" s="141"/>
@@ -23144,7 +23160,7 @@
         <v>751</v>
       </c>
       <c r="F24" s="67" t="s">
-        <v>471</v>
+        <v>607</v>
       </c>
       <c r="G24" s="68" t="s">
         <v>79</v>
@@ -23174,7 +23190,9 @@
       <c r="P24" s="70"/>
       <c r="Q24" s="85"/>
       <c r="R24" s="74"/>
-      <c r="S24" s="73"/>
+      <c r="S24" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U24" s="88"/>
       <c r="V24" s="102"/>
       <c r="W24" s="141"/>
@@ -24201,7 +24219,7 @@
         <v>754</v>
       </c>
       <c r="F25" s="67" t="s">
-        <v>471</v>
+        <v>607</v>
       </c>
       <c r="G25" s="68" t="s">
         <v>79</v>
@@ -24231,7 +24249,9 @@
       <c r="P25" s="70"/>
       <c r="Q25" s="85"/>
       <c r="R25" s="74"/>
-      <c r="S25" s="73"/>
+      <c r="S25" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U25" s="88"/>
       <c r="V25" s="102"/>
       <c r="W25" s="141"/>
@@ -25258,7 +25278,7 @@
         <v>757</v>
       </c>
       <c r="F26" s="67" t="s">
-        <v>456</v>
+        <v>608</v>
       </c>
       <c r="G26" s="68" t="s">
         <v>79</v>
@@ -25288,7 +25308,9 @@
       <c r="P26" s="70"/>
       <c r="Q26" s="85"/>
       <c r="R26" s="74"/>
-      <c r="S26" s="73"/>
+      <c r="S26" s="73" t="s">
+        <v>74</v>
+      </c>
       <c r="U26" s="88"/>
       <c r="V26" s="102"/>
       <c r="W26" s="141"/>
@@ -72479,7 +72501,7 @@
   <dimension ref="A1:AM313"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>